<commit_message>
Test remove hospital outpatient facility [BCIO:026015];
</commit_message>
<xml_diff>
--- a/inputs/AddictO_Environmental_system_Defs.xlsx
+++ b/inputs/AddictO_Environmental_system_Defs.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W44"/>
+  <dimension ref="A1:W43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2288,23 +2288,23 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>BCIO:026015</t>
+          <t>ENVO:00000070</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>hospital outpatient clinic facility</t>
+          <t>human construction</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>A hospital facility to treat patients without them staying overnight, often after a hospital visit.</t>
+          <t>A construction that has been assembled by deliberate human effort.</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
-          <t>hospital facility</t>
+          <t>construction</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2322,17 +2322,13 @@
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>outpatient clinic</t>
-        </is>
-      </c>
+      <c r="M28" t="inlineStr"/>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>true</t>
         </is>
       </c>
       <c r="R28" t="inlineStr">
@@ -2343,7 +2339,7 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" t="inlineStr">
         <is>
-          <t>RW; JH</t>
+          <t>RW</t>
         </is>
       </c>
       <c r="U28" t="inlineStr">
@@ -2355,90 +2351,92 @@
       <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>ENVO:00000070</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>human construction</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>A construction that has been assembled by deliberate human effort.</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>construction</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>material entity</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="inlineStr"/>
-      <c r="N29" t="inlineStr"/>
-      <c r="O29" t="inlineStr"/>
-      <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>ADDICTO:0001280</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>important other</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>A person with whom someone has a sufficiently close relationship that they are willing to discuss important matters.</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr"/>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>person</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="G29" s="2" t="inlineStr"/>
+      <c r="H29" s="2" t="inlineStr"/>
+      <c r="I29" s="2" t="inlineStr"/>
+      <c r="J29" s="2" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K29" s="2" t="inlineStr"/>
+      <c r="L29" s="2" t="inlineStr"/>
+      <c r="M29" s="2" t="inlineStr"/>
+      <c r="N29" s="2" t="inlineStr"/>
+      <c r="O29" s="2" t="inlineStr"/>
+      <c r="P29" s="2" t="inlineStr"/>
+      <c r="Q29" s="2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="R29" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S29" t="inlineStr"/>
-      <c r="T29" t="inlineStr">
+      <c r="R29" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S29" s="2" t="inlineStr">
+        <is>
+          <t>Because it depends on how the term 'important' is judged.</t>
+        </is>
+      </c>
+      <c r="T29" s="2" t="inlineStr">
         <is>
           <t>RW</t>
         </is>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="V29" t="inlineStr"/>
-      <c r="W29" t="inlineStr"/>
+      <c r="U29" s="2" t="inlineStr">
+        <is>
+          <t>Discussed</t>
+        </is>
+      </c>
+      <c r="V29" s="2" t="inlineStr"/>
+      <c r="W29" s="2" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
         <is>
-          <t>ADDICTO:0001280</t>
+          <t>ADDICTO:0001281</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>important other</t>
+          <t>important other who smokes</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>A person with whom someone has a sufficiently close relationship that they are willing to discuss important matters.</t>
+          <t>An important other who smokes tobacco.</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr"/>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>person</t>
+          <t>important other</t>
         </is>
       </c>
       <c r="F30" s="2" t="inlineStr">
@@ -2470,7 +2468,7 @@
       </c>
       <c r="S30" s="2" t="inlineStr">
         <is>
-          <t>Because it depends on how the term 'important' is judged.</t>
+          <t>Because it depends on how the term 'important' is defined.</t>
         </is>
       </c>
       <c r="T30" s="2" t="inlineStr">
@@ -2489,17 +2487,17 @@
     <row r="31">
       <c r="A31" s="2" t="inlineStr">
         <is>
-          <t>ADDICTO:0001281</t>
+          <t>ADDICTO:0001282</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>important other who smokes</t>
+          <t>important other who vapes nicotine</t>
         </is>
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>An important other who smokes tobacco.</t>
+          <t>An important other who vapes nicotine.</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr"/>
@@ -2554,151 +2552,153 @@
       <c r="W31" s="2" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>ADDICTO:0001282</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>important other who vapes nicotine</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>An important other who vapes nicotine.</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="inlineStr"/>
-      <c r="E32" s="2" t="inlineStr">
-        <is>
-          <t>important other</t>
-        </is>
-      </c>
-      <c r="F32" s="2" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="G32" s="2" t="inlineStr"/>
-      <c r="H32" s="2" t="inlineStr"/>
-      <c r="I32" s="2" t="inlineStr"/>
-      <c r="J32" s="2" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K32" s="2" t="inlineStr"/>
-      <c r="L32" s="2" t="inlineStr"/>
-      <c r="M32" s="2" t="inlineStr"/>
-      <c r="N32" s="2" t="inlineStr"/>
-      <c r="O32" s="2" t="inlineStr"/>
-      <c r="P32" s="2" t="inlineStr"/>
-      <c r="Q32" s="2" t="inlineStr">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ENVO:01001406</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>laboratory facility</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>A research facility in which systems of manufactured products control internal conditions and in which scientific or technological research, experiments, and measurement may be performed.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>research facility</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>material entity</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="inlineStr">
+        <is>
+          <t>ADDICTO:0000449</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="inlineStr">
+        <is>
+          <t>level of economic development</t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="inlineStr">
+        <is>
+          <t>A data item that is about the amount and quality of human and physical resources available to the inhabitants of a geospatial region.</t>
+        </is>
+      </c>
+      <c r="D33" s="2" t="inlineStr"/>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>data item</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>generically dependent continuant</t>
+        </is>
+      </c>
+      <c r="G33" s="2" t="inlineStr"/>
+      <c r="H33" s="2" t="inlineStr"/>
+      <c r="I33" s="2" t="inlineStr"/>
+      <c r="J33" s="2" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K33" s="2" t="inlineStr">
+        <is>
+          <t>https://en.wikipedia.org/wiki/Economic_development</t>
+        </is>
+      </c>
+      <c r="L33" s="2" t="inlineStr"/>
+      <c r="M33" s="2" t="inlineStr"/>
+      <c r="N33" s="2" t="inlineStr"/>
+      <c r="O33" s="2" t="inlineStr"/>
+      <c r="P33" s="2" t="inlineStr"/>
+      <c r="Q33" s="2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="R32" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="S32" s="2" t="inlineStr">
-        <is>
-          <t>Because it depends on how the term 'important' is defined.</t>
-        </is>
-      </c>
-      <c r="T32" s="2" t="inlineStr">
+      <c r="R33" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S33" s="2" t="inlineStr"/>
+      <c r="T33" s="2" t="inlineStr">
         <is>
           <t>RW</t>
         </is>
       </c>
-      <c r="U32" s="2" t="inlineStr">
+      <c r="U33" s="2" t="inlineStr">
         <is>
           <t>Discussed</t>
         </is>
       </c>
-      <c r="V32" s="2" t="inlineStr"/>
-      <c r="W32" s="2" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ENVO:01001406</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>laboratory facility</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>A research facility in which systems of manufactured products control internal conditions and in which scientific or technological research, experiments, and measurement may be performed.</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>research facility</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>material entity</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="inlineStr"/>
-      <c r="N33" t="inlineStr"/>
-      <c r="O33" t="inlineStr"/>
-      <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S33" t="inlineStr"/>
-      <c r="T33" t="inlineStr">
-        <is>
-          <t>RW</t>
-        </is>
-      </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="V33" t="inlineStr"/>
-      <c r="W33" t="inlineStr"/>
+      <c r="V33" s="2" t="inlineStr"/>
+      <c r="W33" s="2" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="inlineStr">
         <is>
-          <t>ADDICTO:0000449</t>
+          <t>ADDICTO:0001283</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>level of economic development</t>
+          <t>number of important others in a person's social environment</t>
         </is>
       </c>
       <c r="C34" s="2" t="inlineStr">
         <is>
-          <t>A data item that is about the amount and quality of human and physical resources available to the inhabitants of a geospatial region.</t>
+          <t>A data item that is the number of important others in a person's environmental system.</t>
         </is>
       </c>
       <c r="D34" s="2" t="inlineStr"/>
@@ -2720,11 +2720,7 @@
           <t>Environmental system</t>
         </is>
       </c>
-      <c r="K34" s="2" t="inlineStr">
-        <is>
-          <t>https://en.wikipedia.org/wiki/Economic_development</t>
-        </is>
-      </c>
+      <c r="K34" s="2" t="inlineStr"/>
       <c r="L34" s="2" t="inlineStr"/>
       <c r="M34" s="2" t="inlineStr"/>
       <c r="N34" s="2" t="inlineStr"/>
@@ -2757,17 +2753,17 @@
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>ADDICTO:0001283</t>
+          <t>ADDICTO:0001284</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>number of important others in a person's social environment</t>
+          <t>number of important others who smoke tobacco in a person's social environment.</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>A data item that is the number of important others in a person's environmental system.</t>
+          <t>A data item that is the number of important others who smoke tobacco in a person's social environment.</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr"/>
@@ -2822,17 +2818,17 @@
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>ADDICTO:0001284</t>
+          <t>ADDICTO:0001285</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>number of important others who smoke tobacco in a person's social environment.</t>
+          <t>number of important others who vape nicotine in a person's social environment.</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>A data item that is the number of important others who smoke tobacco in a person's social environment.</t>
+          <t>A data item that is the number of important others who vape nicotine in a person's social environment.</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr"/>
@@ -2885,95 +2881,95 @@
       <c r="W36" s="2" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>ADDICTO:0001285</t>
-        </is>
-      </c>
-      <c r="B37" s="2" t="inlineStr">
-        <is>
-          <t>number of important others who vape nicotine in a person's social environment.</t>
-        </is>
-      </c>
-      <c r="C37" s="2" t="inlineStr">
-        <is>
-          <t>A data item that is the number of important others who vape nicotine in a person's social environment.</t>
-        </is>
-      </c>
-      <c r="D37" s="2" t="inlineStr"/>
-      <c r="E37" s="2" t="inlineStr">
-        <is>
-          <t>data item</t>
-        </is>
-      </c>
-      <c r="F37" s="2" t="inlineStr">
-        <is>
-          <t>generically dependent continuant</t>
-        </is>
-      </c>
-      <c r="G37" s="2" t="inlineStr"/>
-      <c r="H37" s="2" t="inlineStr"/>
-      <c r="I37" s="2" t="inlineStr"/>
-      <c r="J37" s="2" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K37" s="2" t="inlineStr"/>
-      <c r="L37" s="2" t="inlineStr"/>
-      <c r="M37" s="2" t="inlineStr"/>
-      <c r="N37" s="2" t="inlineStr"/>
-      <c r="O37" s="2" t="inlineStr"/>
-      <c r="P37" s="2" t="inlineStr"/>
-      <c r="Q37" s="2" t="inlineStr">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>OMRSE:00000191</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>residential facility</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>A facility that has at least one housing unit as part in which a person or persons live.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>facility</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>material entity</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
+      <c r="Q37" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="R37" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S37" s="2" t="inlineStr"/>
-      <c r="T37" s="2" t="inlineStr">
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr">
         <is>
           <t>RW</t>
         </is>
       </c>
-      <c r="U37" s="2" t="inlineStr">
-        <is>
-          <t>Discussed</t>
-        </is>
-      </c>
-      <c r="V37" s="2" t="inlineStr"/>
-      <c r="W37" s="2" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>External</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>OMRSE:00000191</t>
+          <t>ENVO:00002221</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>residential facility</t>
+          <t>shop</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>A facility that has at least one housing unit as part in which a person or persons live.</t>
+          <t>A commercial building in which a business presents a selection of goods and offers to trade or sell them to customers for money or other goods.</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
-          <t>facility</t>
+          <t>commercial building</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>material entity</t>
+          <t>object</t>
         </is>
       </c>
       <c r="G38" t="inlineStr"/>
@@ -2990,10 +2986,8 @@
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
+      <c r="Q38" t="n">
+        <v>1</v>
       </c>
       <c r="R38" t="inlineStr">
         <is>
@@ -3017,28 +3011,28 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>ENVO:00002221</t>
+          <t>BFO:0000029</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>shop</t>
+          <t>site</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>A commercial building in which a business presents a selection of goods and offers to trade or sell them to customers for money or other goods.</t>
+          <t>A three-dimensional immaterial entity that is (partially or wholly) bounded by a material entity or it is a three-dimensional immaterial part thereof.</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
-          <t>commercial building</t>
+          <t>immaterial entity</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>object</t>
+          <t>site</t>
         </is>
       </c>
       <c r="G39" t="inlineStr"/>
@@ -3055,8 +3049,10 @@
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="n">
-        <v>1</v>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
       </c>
       <c r="R39" t="inlineStr">
         <is>
@@ -3078,331 +3074,266 @@
       <c r="W39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>BFO:0000029</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>A three-dimensional immaterial entity that is (partially or wholly) bounded by a material entity or it is a three-dimensional immaterial part thereof.</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>ADDICTO:0001158</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>social housing</t>
+        </is>
+      </c>
+      <c r="C40" s="3" t="inlineStr">
+        <is>
+          <t>A household residence that is provided for people on low incomes or with particular needs by government agencies or non-profit organizations.</t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr"/>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>household residence</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>material entity</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr"/>
+      <c r="H40" s="3" t="inlineStr"/>
+      <c r="I40" s="3" t="inlineStr"/>
+      <c r="J40" s="3" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K40" s="3" t="inlineStr">
+        <is>
+          <t>https://languages.oup.com/google-dictionary-en/</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr"/>
+      <c r="M40" s="3" t="inlineStr"/>
+      <c r="N40" s="3" t="inlineStr"/>
+      <c r="O40" s="3" t="inlineStr"/>
+      <c r="P40" s="3" t="inlineStr"/>
+      <c r="Q40" s="3" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="R40" s="3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S40" s="3" t="inlineStr"/>
+      <c r="T40" s="3" t="inlineStr">
+        <is>
+          <t>RW</t>
+        </is>
+      </c>
+      <c r="U40" s="3" t="inlineStr">
+        <is>
+          <t>Pre-proposed</t>
+        </is>
+      </c>
+      <c r="V40" s="3" t="inlineStr"/>
+      <c r="W40" s="3" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>BFO:0000006</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>spatial region</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>A continuant entity that is a continuant_part_of spaceR as defined relative to some frame R</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
         <is>
           <t>immaterial entity</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>site</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
-      <c r="M40" t="inlineStr"/>
-      <c r="N40" t="inlineStr"/>
-      <c r="O40" t="inlineStr"/>
-      <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr">
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>spatial region</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
+      <c r="Q41" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="R40" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S40" t="inlineStr"/>
-      <c r="T40" t="inlineStr">
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr">
         <is>
           <t>RW</t>
         </is>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="U41" t="inlineStr">
         <is>
           <t>External</t>
         </is>
       </c>
-      <c r="V40" t="inlineStr"/>
-      <c r="W40" t="inlineStr"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="inlineStr">
-        <is>
-          <t>ADDICTO:0001158</t>
-        </is>
-      </c>
-      <c r="B41" s="3" t="inlineStr">
-        <is>
-          <t>social housing</t>
-        </is>
-      </c>
-      <c r="C41" s="3" t="inlineStr">
-        <is>
-          <t>A household residence that is provided for people on low incomes or with particular needs by government agencies or non-profit organizations.</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="inlineStr"/>
-      <c r="E41" s="3" t="inlineStr">
-        <is>
-          <t>household residence</t>
-        </is>
-      </c>
-      <c r="F41" s="3" t="inlineStr">
-        <is>
-          <t>material entity</t>
-        </is>
-      </c>
-      <c r="G41" s="3" t="inlineStr"/>
-      <c r="H41" s="3" t="inlineStr"/>
-      <c r="I41" s="3" t="inlineStr"/>
-      <c r="J41" s="3" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K41" s="3" t="inlineStr">
-        <is>
-          <t>https://languages.oup.com/google-dictionary-en/</t>
-        </is>
-      </c>
-      <c r="L41" s="3" t="inlineStr"/>
-      <c r="M41" s="3" t="inlineStr"/>
-      <c r="N41" s="3" t="inlineStr"/>
-      <c r="O41" s="3" t="inlineStr"/>
-      <c r="P41" s="3" t="inlineStr"/>
-      <c r="Q41" s="3" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="R41" s="3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S41" s="3" t="inlineStr"/>
-      <c r="T41" s="3" t="inlineStr">
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>ADDICTO:0000440</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>vape shop</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>A shop that primarily sells products related to vaping devices.</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr"/>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>shop</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="inlineStr">
+        <is>
+          <t>object</t>
+        </is>
+      </c>
+      <c r="G42" s="2" t="inlineStr"/>
+      <c r="H42" s="2" t="inlineStr"/>
+      <c r="I42" s="2" t="inlineStr"/>
+      <c r="J42" s="2" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K42" s="2" t="inlineStr"/>
+      <c r="L42" s="2" t="inlineStr"/>
+      <c r="M42" s="2" t="inlineStr"/>
+      <c r="N42" s="2" t="inlineStr"/>
+      <c r="O42" s="2" t="inlineStr"/>
+      <c r="P42" s="2" t="inlineStr"/>
+      <c r="Q42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="R42" s="2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S42" s="2" t="inlineStr"/>
+      <c r="T42" s="2" t="inlineStr">
         <is>
           <t>RW</t>
         </is>
       </c>
-      <c r="U41" s="3" t="inlineStr">
-        <is>
-          <t>Pre-proposed</t>
-        </is>
-      </c>
-      <c r="V41" s="3" t="inlineStr"/>
-      <c r="W41" s="3" t="inlineStr"/>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>BFO:0000006</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>spatial region</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>A continuant entity that is a continuant_part_of spaceR as defined relative to some frame R</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr">
+      <c r="U42" s="2" t="inlineStr">
+        <is>
+          <t>Discussed</t>
+        </is>
+      </c>
+      <c r="V42" s="2" t="inlineStr"/>
+      <c r="W42" s="2" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>BCIO:026002</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>within-country location</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>A geographical location within a country where the intervention takes place.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>geographic location</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
         <is>
           <t>immaterial entity</t>
         </is>
       </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>spatial region</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
-      <c r="M42" t="inlineStr"/>
-      <c r="N42" t="inlineStr"/>
-      <c r="O42" t="inlineStr"/>
-      <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-      <c r="R42" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S42" t="inlineStr"/>
-      <c r="T42" t="inlineStr">
-        <is>
-          <t>RW</t>
-        </is>
-      </c>
-      <c r="U42" t="inlineStr">
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Environmental system</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>RW; BG</t>
+        </is>
+      </c>
+      <c r="U43" t="inlineStr">
         <is>
           <t>External</t>
         </is>
       </c>
-      <c r="V42" t="inlineStr"/>
-      <c r="W42" t="inlineStr"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="inlineStr">
-        <is>
-          <t>ADDICTO:0000440</t>
-        </is>
-      </c>
-      <c r="B43" s="2" t="inlineStr">
-        <is>
-          <t>vape shop</t>
-        </is>
-      </c>
-      <c r="C43" s="2" t="inlineStr">
-        <is>
-          <t>A shop that primarily sells products related to vaping devices.</t>
-        </is>
-      </c>
-      <c r="D43" s="2" t="inlineStr"/>
-      <c r="E43" s="2" t="inlineStr">
-        <is>
-          <t>shop</t>
-        </is>
-      </c>
-      <c r="F43" s="2" t="inlineStr">
-        <is>
-          <t>object</t>
-        </is>
-      </c>
-      <c r="G43" s="2" t="inlineStr"/>
-      <c r="H43" s="2" t="inlineStr"/>
-      <c r="I43" s="2" t="inlineStr"/>
-      <c r="J43" s="2" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K43" s="2" t="inlineStr"/>
-      <c r="L43" s="2" t="inlineStr"/>
-      <c r="M43" s="2" t="inlineStr"/>
-      <c r="N43" s="2" t="inlineStr"/>
-      <c r="O43" s="2" t="inlineStr"/>
-      <c r="P43" s="2" t="inlineStr"/>
-      <c r="Q43" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="R43" s="2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S43" s="2" t="inlineStr"/>
-      <c r="T43" s="2" t="inlineStr">
-        <is>
-          <t>RW</t>
-        </is>
-      </c>
-      <c r="U43" s="2" t="inlineStr">
-        <is>
-          <t>Discussed</t>
-        </is>
-      </c>
-      <c r="V43" s="2" t="inlineStr"/>
-      <c r="W43" s="2" t="inlineStr"/>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>BCIO:026002</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>within-country location</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>A geographical location within a country where the intervention takes place.</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>geographic location</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>immaterial entity</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr"/>
-      <c r="H44" t="inlineStr"/>
-      <c r="I44" t="inlineStr"/>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>Environmental system</t>
-        </is>
-      </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="inlineStr"/>
-      <c r="N44" t="inlineStr"/>
-      <c r="O44" t="inlineStr"/>
-      <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="R44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="S44" t="inlineStr"/>
-      <c r="T44" t="inlineStr">
-        <is>
-          <t>RW; BG</t>
-        </is>
-      </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>External</t>
-        </is>
-      </c>
-      <c r="V44" t="inlineStr"/>
-      <c r="W44" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>